<commit_message>
removed created by in import jurnal
</commit_message>
<xml_diff>
--- a/public/contoh-excel/jurnal.xlsx
+++ b/public/contoh-excel/jurnal.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>periode_jurnal</t>
   </si>
@@ -37,22 +37,19 @@
     <t>kredit</t>
   </si>
   <si>
-    <t>created_by</t>
-  </si>
-  <si>
     <t>2023-12-12</t>
   </si>
   <si>
     <t>ju</t>
   </si>
   <si>
-    <t>Pembelian Canang Banten</t>
+    <t>Pembelian AC</t>
   </si>
   <si>
     <t>BK-900</t>
   </si>
   <si>
-    <t>Bank BRI</t>
+    <t>Bank BNI</t>
   </si>
 </sst>
 </file>
@@ -997,19 +994,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="17.5" style="1" customWidth="true"/>
     <col min="4" max="4" width="25.9" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,60 +1028,51 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
       <c r="F2">
-        <v>50000</v>
+        <v>1500000</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>50000</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+        <v>1500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>